<commit_message>
adding motor vehicle component
</commit_message>
<xml_diff>
--- a/rsmsa/public/uploads/driver.xlsx
+++ b/rsmsa/public/uploads/driver.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="30">
   <si>
     <t>Surname</t>
   </si>
@@ -101,7 +101,10 @@
     <t>Bussines</t>
   </si>
   <si>
-    <t>C</t>
+    <t>D,C</t>
+  </si>
+  <si>
+    <t>D,B</t>
   </si>
 </sst>
 </file>
@@ -280,10 +283,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -402,7 +405,7 @@
         <v>929839</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>7823782</v>
+        <v>7283749</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>17</v>
@@ -420,9 +423,173 @@
         <v>27</v>
       </c>
       <c r="L3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>42194</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>929839</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>7283750</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>92839830</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="2" t="n">
+      <c r="M4" s="2" t="n">
+        <v>42194</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>929839</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>7283751</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>92839831</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>42194</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>929839</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>7283752</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>92839832</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>42194</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>929839</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>7283753</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>92839833</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="2" t="n">
         <v>42194</v>
       </c>
     </row>

</xml_diff>